<commit_message>
definition changes adding caseworker-caa role for 8811 tests
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/462450/IdeaProjects/ccd-data-store-api/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0424671-C5AE-D04B-BC29-26AC02A59927}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4325C90D-0404-534C-98C4-4DD9FE1DAF2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" tabRatio="823" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" tabRatio="823" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="195">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -646,6 +646,9 @@
   </si>
   <si>
     <t>CT With No Cases -Don't Create</t>
+  </si>
+  <si>
+    <t>caseworker-caa</t>
   </si>
 </sst>
 </file>
@@ -2776,8 +2779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2858,10 +2861,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2917,33 +2920,48 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="29">
         <v>43466</v>
       </c>
       <c r="B4" s="24"/>
-      <c r="C4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>188</v>
+      <c r="C4" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>194</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="29">
         <v>43466</v>
       </c>
       <c r="B5" s="24"/>
-      <c r="C5" s="14" t="s">
-        <v>191</v>
+      <c r="C5" t="s">
+        <v>186</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>188</v>
       </c>
       <c r="E5" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A6" s="29">
+        <v>43466</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2960,10 +2978,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD9"/>
+      <selection activeCell="E5" sqref="E5:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3034,14 +3052,14 @@
         <v>43466</v>
       </c>
       <c r="B4" s="53"/>
-      <c r="C4" t="s">
+      <c r="C4" s="14" t="s">
         <v>186</v>
       </c>
       <c r="D4" s="42" t="s">
         <v>149</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F4" s="73" t="s">
         <v>120</v>
@@ -3059,7 +3077,7 @@
         <v>150</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F5" s="73" t="s">
         <v>120</v>
@@ -3077,7 +3095,7 @@
         <v>153</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F6" s="73" t="s">
         <v>120</v>
@@ -3088,8 +3106,8 @@
         <v>43466</v>
       </c>
       <c r="B7" s="53"/>
-      <c r="C7" s="14" t="s">
-        <v>191</v>
+      <c r="C7" t="s">
+        <v>186</v>
       </c>
       <c r="D7" s="42" t="s">
         <v>149</v>
@@ -3107,7 +3125,7 @@
       </c>
       <c r="B8" s="53"/>
       <c r="C8" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D8" s="42" t="s">
         <v>150</v>
@@ -3125,7 +3143,7 @@
       </c>
       <c r="B9" s="53"/>
       <c r="C9" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D9" s="42" t="s">
         <v>153</v>
@@ -3134,6 +3152,60 @@
         <v>188</v>
       </c>
       <c r="F9" s="73" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="59">
+        <v>43466</v>
+      </c>
+      <c r="B10" s="53"/>
+      <c r="C10" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="E10" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" s="73" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="59">
+        <v>43466</v>
+      </c>
+      <c r="B11" s="53"/>
+      <c r="C11" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="E11" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="73" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="59">
+        <v>43466</v>
+      </c>
+      <c r="B12" s="53"/>
+      <c r="C12" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" s="73" t="s">
         <v>120</v>
       </c>
     </row>
@@ -3150,10 +3222,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD15"/>
+      <selection activeCell="E4" sqref="E4:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3221,14 +3293,14 @@
       <c r="A4" s="72">
         <v>43466</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="14" t="s">
         <v>186</v>
       </c>
       <c r="D4" s="42" t="s">
         <v>154</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>120</v>
@@ -3245,7 +3317,7 @@
         <v>156</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>120</v>
@@ -3262,7 +3334,7 @@
         <v>158</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>120</v>
@@ -3279,7 +3351,7 @@
         <v>160</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F7" s="24" t="s">
         <v>120</v>
@@ -3296,7 +3368,7 @@
         <v>162</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F8" s="24" t="s">
         <v>120</v>
@@ -3313,7 +3385,7 @@
         <v>170</v>
       </c>
       <c r="E9" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>120</v>
@@ -3323,8 +3395,8 @@
       <c r="A10" s="72">
         <v>43466</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>191</v>
+      <c r="C10" t="s">
+        <v>186</v>
       </c>
       <c r="D10" s="42" t="s">
         <v>154</v>
@@ -3341,7 +3413,7 @@
         <v>43466</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D11" s="42" t="s">
         <v>156</v>
@@ -3358,7 +3430,7 @@
         <v>43466</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D12" s="42" t="s">
         <v>158</v>
@@ -3375,7 +3447,7 @@
         <v>43466</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D13" s="42" t="s">
         <v>160</v>
@@ -3392,7 +3464,7 @@
         <v>43466</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D14" s="42" t="s">
         <v>162</v>
@@ -3409,7 +3481,7 @@
         <v>43466</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D15" s="42" t="s">
         <v>170</v>
@@ -3418,6 +3490,108 @@
         <v>188</v>
       </c>
       <c r="F15" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E16" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E19" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E21" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F21" s="24" t="s">
         <v>120</v>
       </c>
     </row>
@@ -3434,10 +3608,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD15"/>
+      <selection activeCell="E4" sqref="E4:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3500,18 +3674,18 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="72">
         <v>43466</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="14" t="s">
         <v>186</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>130</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>120</v>
@@ -3528,7 +3702,7 @@
         <v>132</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>120</v>
@@ -3545,7 +3719,7 @@
         <v>134</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>120</v>
@@ -3562,7 +3736,7 @@
         <v>139</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F7" s="24" t="s">
         <v>120</v>
@@ -3579,7 +3753,7 @@
         <v>141</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F8" s="24" t="s">
         <v>120</v>
@@ -3596,18 +3770,18 @@
         <v>145</v>
       </c>
       <c r="E9" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="72">
         <v>43466</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>191</v>
+      <c r="C10" t="s">
+        <v>186</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>130</v>
@@ -3624,7 +3798,7 @@
         <v>43466</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D11" s="28" t="s">
         <v>132</v>
@@ -3641,7 +3815,7 @@
         <v>43466</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>134</v>
@@ -3658,7 +3832,7 @@
         <v>43466</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D13" s="42" t="s">
         <v>139</v>
@@ -3675,7 +3849,7 @@
         <v>43466</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D14" s="42" t="s">
         <v>141</v>
@@ -3692,7 +3866,7 @@
         <v>43466</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D15" s="42" t="s">
         <v>145</v>
@@ -3704,55 +3878,127 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="72"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="24"/>
+    <row r="16" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="17" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="72"/>
-      <c r="D17" s="42"/>
-      <c r="F17" s="24"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="72"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="24"/>
+      <c r="A17" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="E18" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="19" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="72"/>
-      <c r="D19" s="42"/>
-      <c r="F19" s="24"/>
+      <c r="A19" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="E19" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="20" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="72"/>
-      <c r="D20" s="42"/>
-      <c r="F20" s="24"/>
+      <c r="A20" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="21" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="72"/>
-      <c r="D21" s="28"/>
-      <c r="F21" s="24"/>
-    </row>
-    <row r="22" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="72">
+        <v>43466</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="E21" s="60" t="s">
+        <v>188</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="72"/>
-      <c r="D22" s="28"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="14"/>
       <c r="F22" s="24"/>
     </row>
     <row r="23" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="72"/>
-      <c r="D23" s="28"/>
+      <c r="D23" s="42"/>
       <c r="F23" s="24"/>
     </row>
-    <row r="24" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="72"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="42"/>
+      <c r="E24" s="14"/>
       <c r="F24" s="24"/>
     </row>
     <row r="25" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3767,17 +4013,17 @@
     </row>
     <row r="27" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="72"/>
-      <c r="D27" s="42"/>
+      <c r="D27" s="28"/>
       <c r="F27" s="24"/>
     </row>
     <row r="28" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="72"/>
-      <c r="D28" s="42"/>
+      <c r="D28" s="28"/>
       <c r="F28" s="24"/>
     </row>
     <row r="29" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="72"/>
-      <c r="D29" s="42"/>
+      <c r="D29" s="28"/>
       <c r="F29" s="24"/>
     </row>
     <row r="30" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3792,7 +4038,7 @@
     </row>
     <row r="32" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="72"/>
-      <c r="D32" s="24"/>
+      <c r="D32" s="42"/>
       <c r="F32" s="24"/>
     </row>
     <row r="33" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3814,6 +4060,36 @@
       <c r="A36" s="72"/>
       <c r="D36" s="42"/>
       <c r="F36" s="24"/>
+    </row>
+    <row r="37" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="72"/>
+      <c r="D37" s="42"/>
+      <c r="F37" s="24"/>
+    </row>
+    <row r="38" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="72"/>
+      <c r="D38" s="24"/>
+      <c r="F38" s="24"/>
+    </row>
+    <row r="39" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="72"/>
+      <c r="D39" s="42"/>
+      <c r="F39" s="24"/>
+    </row>
+    <row r="40" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="72"/>
+      <c r="D40" s="42"/>
+      <c r="F40" s="24"/>
+    </row>
+    <row r="41" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="72"/>
+      <c r="D41" s="42"/>
+      <c r="F41" s="24"/>
+    </row>
+    <row r="42" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="72"/>
+      <c r="D42" s="42"/>
+      <c r="F42" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RDM-11029: Have two different roles for fields
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="198">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -513,6 +513,9 @@
   </si>
   <si>
     <t>UserRole</t>
+  </si>
+  <si>
+    <t>pui-caa</t>
   </si>
   <si>
     <t>caseworker-befta_jurisdiction_1</t>
@@ -3044,7 +3047,9 @@
       <c r="C4" t="s" s="13">
         <v>24</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" t="s" s="13">
+        <v>158</v>
+      </c>
       <c r="E4" t="s" s="13">
         <v>47</v>
       </c>
@@ -3063,7 +3068,9 @@
       <c r="C5" t="s" s="13">
         <v>24</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" t="s" s="13">
+        <v>158</v>
+      </c>
       <c r="E5" t="s" s="13">
         <v>64</v>
       </c>
@@ -3121,13 +3128,13 @@
         <v>24</v>
       </c>
       <c r="D8" t="s" s="13">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E8" t="s" s="13">
         <v>47</v>
       </c>
       <c r="F8" t="s" s="13">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G8" s="33">
         <v>1</v>
@@ -3142,13 +3149,13 @@
         <v>24</v>
       </c>
       <c r="D9" t="s" s="13">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E9" t="s" s="13">
         <v>64</v>
       </c>
       <c r="F9" t="s" s="13">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G9" s="33">
         <v>2</v>
@@ -3198,7 +3205,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B1" s="74"/>
       <c r="C1" t="s" s="10">
@@ -3228,16 +3235,16 @@
         <v>4</v>
       </c>
       <c r="F2" t="s" s="13">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G2" t="s" s="13">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H2" t="s" s="13">
         <v>4</v>
       </c>
       <c r="I2" t="s" s="13">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
@@ -3251,22 +3258,22 @@
         <v>38</v>
       </c>
       <c r="D3" t="s" s="10">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E3" t="s" s="10">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F3" t="s" s="9">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G3" t="s" s="9">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H3" t="s" s="32">
         <v>130</v>
       </c>
       <c r="I3" t="s" s="9">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
@@ -3278,13 +3285,13 @@
         <v>24</v>
       </c>
       <c r="D4" t="s" s="13">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E4" t="s" s="13">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F4" t="s" s="48">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G4" s="33">
         <v>1</v>
@@ -3305,13 +3312,13 @@
         <v>24</v>
       </c>
       <c r="D5" t="s" s="13">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E5" t="s" s="13">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F5" t="s" s="48">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G5" s="33">
         <v>1</v>
@@ -3332,13 +3339,13 @@
         <v>24</v>
       </c>
       <c r="D6" t="s" s="13">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E6" t="s" s="13">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F6" t="s" s="48">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G6" s="33">
         <v>1</v>
@@ -3359,13 +3366,13 @@
         <v>24</v>
       </c>
       <c r="D7" t="s" s="13">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E7" t="s" s="13">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F7" t="s" s="48">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G7" s="33">
         <v>1</v>
@@ -3386,13 +3393,13 @@
         <v>24</v>
       </c>
       <c r="D8" t="s" s="13">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E8" t="s" s="13">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F8" t="s" s="48">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G8" s="33">
         <v>1</v>
@@ -3413,13 +3420,13 @@
         <v>24</v>
       </c>
       <c r="D9" t="s" s="13">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E9" t="s" s="13">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F9" t="s" s="48">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G9" s="33">
         <v>2</v>
@@ -3440,13 +3447,13 @@
         <v>28</v>
       </c>
       <c r="D10" t="s" s="13">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E10" t="s" s="13">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F10" t="s" s="48">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G10" s="33">
         <v>1</v>
@@ -3467,13 +3474,13 @@
         <v>28</v>
       </c>
       <c r="D11" t="s" s="13">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E11" t="s" s="13">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F11" t="s" s="48">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G11" s="33">
         <v>1</v>
@@ -3494,13 +3501,13 @@
         <v>28</v>
       </c>
       <c r="D12" t="s" s="13">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E12" t="s" s="13">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F12" t="s" s="48">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G12" s="33">
         <v>1</v>
@@ -3521,13 +3528,13 @@
         <v>28</v>
       </c>
       <c r="D13" t="s" s="13">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E13" t="s" s="13">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F13" t="s" s="48">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G13" s="33">
         <v>1</v>
@@ -3548,13 +3555,13 @@
         <v>28</v>
       </c>
       <c r="D14" t="s" s="13">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E14" t="s" s="13">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F14" t="s" s="48">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G14" s="33">
         <v>1</v>
@@ -3575,13 +3582,13 @@
         <v>28</v>
       </c>
       <c r="D15" t="s" s="13">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E15" t="s" s="13">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F15" t="s" s="48">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G15" s="33">
         <v>2</v>
@@ -3852,7 +3859,7 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s" s="3">
         <v>1</v>
@@ -3882,16 +3889,16 @@
         <v>8</v>
       </c>
       <c r="C3" t="s" s="10">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D3" t="s" s="78">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E3" t="s" s="78">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F3" t="s" s="16">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1">
@@ -3900,7 +3907,7 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" t="s" s="13">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D4" t="s" s="43">
         <v>12</v>
@@ -3990,7 +3997,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B1" t="s" s="3">
         <v>1</v>
@@ -4010,10 +4017,10 @@
         <v>4</v>
       </c>
       <c r="D2" t="s" s="8">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E2" t="s" s="8">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" ht="13" customHeight="1">
@@ -4030,7 +4037,7 @@
         <v>157</v>
       </c>
       <c r="E3" t="s" s="9">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" ht="13" customHeight="1">
@@ -4042,10 +4049,10 @@
         <v>24</v>
       </c>
       <c r="D4" t="s" s="13">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E4" t="s" s="13">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" ht="13" customHeight="1">
@@ -4057,10 +4064,10 @@
         <v>24</v>
       </c>
       <c r="D5" t="s" s="13">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E5" t="s" s="13">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" ht="13" customHeight="1">
@@ -4072,10 +4079,10 @@
         <v>28</v>
       </c>
       <c r="D6" t="s" s="13">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E6" t="s" s="13">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" ht="13.65" customHeight="1">
@@ -4134,7 +4141,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="82">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B1" t="s" s="83">
         <v>1</v>
@@ -4158,10 +4165,10 @@
         <v>4</v>
       </c>
       <c r="E2" t="s" s="88">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F2" t="s" s="88">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" ht="13" customHeight="1">
@@ -4175,13 +4182,13 @@
         <v>38</v>
       </c>
       <c r="D3" t="s" s="89">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E3" t="s" s="89">
         <v>157</v>
       </c>
       <c r="F3" t="s" s="40">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" ht="13" customHeight="1">
@@ -4196,10 +4203,10 @@
         <v>83</v>
       </c>
       <c r="E4" t="s" s="93">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F4" t="s" s="94">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" ht="13" customHeight="1">
@@ -4214,10 +4221,10 @@
         <v>85</v>
       </c>
       <c r="E5" t="s" s="97">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F5" t="s" s="94">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" ht="13" customHeight="1">
@@ -4232,10 +4239,10 @@
         <v>87</v>
       </c>
       <c r="E6" t="s" s="97">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F6" t="s" s="94">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" ht="13" customHeight="1">
@@ -4250,10 +4257,10 @@
         <v>83</v>
       </c>
       <c r="E7" t="s" s="97">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F7" t="s" s="94">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" ht="13" customHeight="1">
@@ -4268,10 +4275,10 @@
         <v>85</v>
       </c>
       <c r="E8" t="s" s="97">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F8" t="s" s="94">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" ht="13" customHeight="1">
@@ -4286,10 +4293,10 @@
         <v>87</v>
       </c>
       <c r="E9" t="s" s="97">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F9" t="s" s="94">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" ht="13" customHeight="1">
@@ -4304,10 +4311,10 @@
         <v>83</v>
       </c>
       <c r="E10" t="s" s="97">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F10" t="s" s="94">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" ht="13" customHeight="1">
@@ -4322,10 +4329,10 @@
         <v>85</v>
       </c>
       <c r="E11" t="s" s="97">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F11" t="s" s="94">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" ht="13" customHeight="1">
@@ -4340,10 +4347,10 @@
         <v>87</v>
       </c>
       <c r="E12" t="s" s="98">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F12" t="s" s="94">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -4374,7 +4381,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B1" t="s" s="3">
         <v>1</v>
@@ -4398,10 +4405,10 @@
         <v>4</v>
       </c>
       <c r="E2" t="s" s="8">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F2" t="s" s="8">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" ht="13" customHeight="1">
@@ -4421,7 +4428,7 @@
         <v>157</v>
       </c>
       <c r="F3" t="s" s="13">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
@@ -4436,10 +4443,10 @@
         <v>105</v>
       </c>
       <c r="E4" t="s" s="102">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F4" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
@@ -4454,10 +4461,10 @@
         <v>108</v>
       </c>
       <c r="E5" t="s" s="102">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F5" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
@@ -4472,10 +4479,10 @@
         <v>110</v>
       </c>
       <c r="E6" t="s" s="102">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F6" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
@@ -4490,10 +4497,10 @@
         <v>112</v>
       </c>
       <c r="E7" t="s" s="102">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F7" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
@@ -4508,10 +4515,10 @@
         <v>114</v>
       </c>
       <c r="E8" t="s" s="102">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F8" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
@@ -4526,10 +4533,10 @@
         <v>117</v>
       </c>
       <c r="E9" t="s" s="102">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F9" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -4544,10 +4551,10 @@
         <v>105</v>
       </c>
       <c r="E10" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F10" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
@@ -4562,10 +4569,10 @@
         <v>108</v>
       </c>
       <c r="E11" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F11" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
@@ -4580,10 +4587,10 @@
         <v>110</v>
       </c>
       <c r="E12" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F12" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1">
@@ -4598,10 +4605,10 @@
         <v>112</v>
       </c>
       <c r="E13" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F13" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1">
@@ -4616,10 +4623,10 @@
         <v>114</v>
       </c>
       <c r="E14" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F14" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1">
@@ -4634,10 +4641,10 @@
         <v>117</v>
       </c>
       <c r="E15" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F15" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1">
@@ -4652,10 +4659,10 @@
         <v>105</v>
       </c>
       <c r="E16" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F16" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1">
@@ -4670,10 +4677,10 @@
         <v>108</v>
       </c>
       <c r="E17" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F17" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1">
@@ -4688,10 +4695,10 @@
         <v>110</v>
       </c>
       <c r="E18" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F18" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1">
@@ -4706,10 +4713,10 @@
         <v>112</v>
       </c>
       <c r="E19" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F19" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1">
@@ -4724,10 +4731,10 @@
         <v>114</v>
       </c>
       <c r="E20" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F20" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1">
@@ -4742,10 +4749,10 @@
         <v>117</v>
       </c>
       <c r="E21" t="s" s="104">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F21" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -4776,7 +4783,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B1" t="s" s="3">
         <v>1</v>
@@ -4803,7 +4810,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s" s="27">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" ht="13" customHeight="1">
@@ -4823,7 +4830,7 @@
         <v>157</v>
       </c>
       <c r="F3" t="s" s="13">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
@@ -4838,10 +4845,10 @@
         <v>47</v>
       </c>
       <c r="E4" t="s" s="102">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F4" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
@@ -4856,10 +4863,10 @@
         <v>52</v>
       </c>
       <c r="E5" t="s" s="102">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F5" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
@@ -4874,10 +4881,10 @@
         <v>56</v>
       </c>
       <c r="E6" t="s" s="102">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F6" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
@@ -4892,10 +4899,10 @@
         <v>60</v>
       </c>
       <c r="E7" t="s" s="102">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F7" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
@@ -4910,10 +4917,10 @@
         <v>64</v>
       </c>
       <c r="E8" t="s" s="102">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F8" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
@@ -4928,10 +4935,10 @@
         <v>68</v>
       </c>
       <c r="E9" t="s" s="102">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F9" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -4946,10 +4953,10 @@
         <v>47</v>
       </c>
       <c r="E10" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F10" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
@@ -4964,10 +4971,10 @@
         <v>52</v>
       </c>
       <c r="E11" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F11" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
@@ -4982,10 +4989,10 @@
         <v>56</v>
       </c>
       <c r="E12" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F12" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1">
@@ -5000,10 +5007,10 @@
         <v>60</v>
       </c>
       <c r="E13" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F13" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1">
@@ -5018,10 +5025,10 @@
         <v>64</v>
       </c>
       <c r="E14" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F14" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1">
@@ -5036,10 +5043,10 @@
         <v>68</v>
       </c>
       <c r="E15" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F15" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1">
@@ -5054,10 +5061,10 @@
         <v>47</v>
       </c>
       <c r="E16" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F16" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1">
@@ -5072,10 +5079,10 @@
         <v>52</v>
       </c>
       <c r="E17" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F17" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1">
@@ -5090,10 +5097,10 @@
         <v>56</v>
       </c>
       <c r="E18" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F18" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1">
@@ -5108,10 +5115,10 @@
         <v>60</v>
       </c>
       <c r="E19" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F19" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1">
@@ -5126,10 +5133,10 @@
         <v>64</v>
       </c>
       <c r="E20" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F20" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1">
@@ -5144,10 +5151,10 @@
         <v>68</v>
       </c>
       <c r="E21" t="s" s="102">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F21" t="s" s="103">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1">
@@ -5347,7 +5354,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="108">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B1" t="s" s="109">
         <v>1</v>
@@ -5366,19 +5373,19 @@
       <c r="A2" s="35"/>
       <c r="B2" s="35"/>
       <c r="C2" t="s" s="27">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D2" t="s" s="27">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E2" t="s" s="27">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F2" t="s" s="27">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G2" t="s" s="27">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" ht="13.65" customHeight="1">
@@ -5401,7 +5408,7 @@
         <v>157</v>
       </c>
       <c r="G3" t="s" s="28">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1">

</xml_diff>